<commit_message>
ajout des perfs dans le xls
</commit_message>
<xml_diff>
--- a/doc/Classeur.xlsx
+++ b/doc/Classeur.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="240" yWindow="120" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
+    <sheet name="50 repliques" sheetId="1" r:id="rId1"/>
+    <sheet name="5000 repliques" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="10">
   <si>
     <t>max</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Données</t>
+  </si>
+  <si>
+    <t>Replications</t>
+  </si>
+  <si>
+    <t>Temps (s)</t>
   </si>
 </sst>
 </file>
@@ -78,15 +84,22 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -94,6 +107,284 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="fr-FR"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="140"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="40"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:trendline>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout>
+                <c:manualLayout>
+                  <c:x val="-2.7812992125984252E-2"/>
+                  <c:y val="-2.8252405949256341E-2"/>
+                </c:manualLayout>
+              </c:layout>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Feuil3!$A$2:$A$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>200</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>300</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>400</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>500</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>600</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>700</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>800</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>900</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5000</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Feuil3!$B$2:$B$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="20"/>
+                <c:pt idx="0">
+                  <c:v>0.34799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.53200000000000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.02</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.94399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.016</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.8159999999999998</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.8119999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.6760000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>6.8959999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>10.521000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>11.541</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>14.605</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>18.844999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.972999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>22.516999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>26.373999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>27.998000000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>125</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="146540800"/>
+        <c:axId val="146538880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="146540800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146538880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="146538880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="146540800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>757237</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>757237</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Graphique 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:B21" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A1:B21"/>
+  <tableColumns count="2">
+    <tableColumn id="1" name="Replications"/>
+    <tableColumn id="2" name="Temps (s)"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -386,7 +677,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25781,12 +26072,191 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="14" customWidth="1"/>
+    <col min="2" max="2" width="11.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.34799999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>0.53200000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>1.02</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0.94399999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>1.44</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>2.016</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>80</v>
+      </c>
+      <c r="B9">
+        <v>2.8159999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>90</v>
+      </c>
+      <c r="B10">
+        <v>2.8119999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>100</v>
+      </c>
+      <c r="B11">
+        <v>3.6760000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>200</v>
+      </c>
+      <c r="B12">
+        <v>6.8959999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>300</v>
+      </c>
+      <c r="B13">
+        <v>10.521000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>400</v>
+      </c>
+      <c r="B14">
+        <v>11.541</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>500</v>
+      </c>
+      <c r="B15">
+        <v>14.605</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>600</v>
+      </c>
+      <c r="B16">
+        <v>18.844999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>700</v>
+      </c>
+      <c r="B17">
+        <v>19.972999999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>800</v>
+      </c>
+      <c r="B18">
+        <v>22.516999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>900</v>
+      </c>
+      <c r="B19">
+        <v>26.373999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>1000</v>
+      </c>
+      <c r="B20">
+        <v>27.998000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>5000</v>
+      </c>
+      <c r="B21">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>